<commit_message>
added local mixing experiment of ash layer
</commit_message>
<xml_diff>
--- a/data/iTURBO2_input_ash_experiment.xlsx
+++ b/data/iTURBO2_input_ash_experiment.xlsx
@@ -144,7 +144,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +154,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFF200"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
@@ -241,7 +247,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -302,6 +308,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -359,7 +377,7 @@
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -402,7 +420,7 @@
   <dimension ref="A1:Z104"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+      <selection pane="topLeft" activeCell="P30" activeCellId="0" sqref="P30:Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -414,7 +432,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.81"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="11.52"/>
@@ -1441,24 +1459,24 @@
       <c r="N18" s="14" t="n">
         <v>0.03</v>
       </c>
-      <c r="O18" s="11" t="n">
+      <c r="O18" s="15" t="n">
         <v>104</v>
       </c>
-      <c r="P18" s="0" t="n">
+      <c r="P18" s="16" t="n">
         <f aca="false">+O18-69</f>
         <v>35</v>
       </c>
-      <c r="Q18" s="14" t="n">
+      <c r="Q18" s="17" t="n">
         <v>0.16</v>
       </c>
-      <c r="R18" s="11" t="n">
+      <c r="R18" s="15" t="n">
         <v>337</v>
       </c>
-      <c r="S18" s="0" t="n">
+      <c r="S18" s="16" t="n">
         <f aca="false">+R18-295</f>
         <v>42</v>
       </c>
-      <c r="T18" s="14" t="n">
+      <c r="T18" s="17" t="n">
         <v>0.072</v>
       </c>
       <c r="U18" s="11" t="n">
@@ -1528,14 +1546,14 @@
       <c r="Q19" s="14" t="n">
         <v>0.05</v>
       </c>
-      <c r="R19" s="11" t="n">
+      <c r="R19" s="15" t="n">
         <v>339</v>
       </c>
-      <c r="S19" s="0" t="n">
+      <c r="S19" s="16" t="n">
         <f aca="false">+R19-295</f>
         <v>44</v>
       </c>
-      <c r="T19" s="14" t="n">
+      <c r="T19" s="17" t="n">
         <v>0.073</v>
       </c>
       <c r="U19" s="11" t="n">
@@ -2027,22 +2045,22 @@
       <c r="K28" s="14"/>
       <c r="L28" s="11"/>
       <c r="N28" s="14"/>
-      <c r="O28" s="15" t="s">
+      <c r="O28" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
-      <c r="U28" s="15" t="s">
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="18"/>
+      <c r="U28" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="V28" s="15"/>
-      <c r="W28" s="15"/>
-      <c r="X28" s="15"/>
-      <c r="Y28" s="15"/>
-      <c r="Z28" s="15"/>
+      <c r="V28" s="18"/>
+      <c r="W28" s="18"/>
+      <c r="X28" s="18"/>
+      <c r="Y28" s="18"/>
+      <c r="Z28" s="18"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="n">
@@ -2988,14 +3006,14 @@
       <c r="K41" s="14" t="n">
         <v>0.002</v>
       </c>
-      <c r="L41" s="16" t="n">
+      <c r="L41" s="19" t="n">
         <v>692</v>
       </c>
       <c r="M41" s="0" t="n">
         <f aca="false">L41-L$37</f>
         <v>18</v>
       </c>
-      <c r="N41" s="17" t="n">
+      <c r="N41" s="20" t="n">
         <v>0.001</v>
       </c>
       <c r="O41" s="11" t="n">
@@ -3055,19 +3073,19 @@
       <c r="F42" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I42" s="16" t="n">
+      <c r="I42" s="19" t="n">
         <v>472</v>
       </c>
       <c r="J42" s="0" t="n">
         <f aca="false">I42-I$36</f>
         <v>15</v>
       </c>
-      <c r="K42" s="17" t="n">
+      <c r="K42" s="20" t="n">
         <v>0.002</v>
       </c>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
       <c r="O42" s="11" t="n">
         <v>118</v>
       </c>
@@ -3125,24 +3143,24 @@
       <c r="F43" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="O43" s="16" t="n">
+      <c r="O43" s="19" t="n">
         <v>124</v>
       </c>
       <c r="P43" s="0" t="n">
         <f aca="false">O43-O$38</f>
         <v>20</v>
       </c>
-      <c r="Q43" s="17" t="n">
+      <c r="Q43" s="20" t="n">
         <v>0.003</v>
       </c>
-      <c r="R43" s="16" t="n">
+      <c r="R43" s="19" t="n">
         <v>355</v>
       </c>
       <c r="S43" s="0" t="n">
         <f aca="false">R43-R$39</f>
         <v>16</v>
       </c>
-      <c r="T43" s="17" t="n">
+      <c r="T43" s="20" t="n">
         <v>0.003</v>
       </c>
       <c r="U43" s="11" t="n">
@@ -3231,14 +3249,14 @@
       <c r="F45" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="U45" s="16" t="n">
+      <c r="U45" s="19" t="n">
         <v>160</v>
       </c>
       <c r="V45" s="0" t="n">
         <f aca="false">U45-U$37</f>
         <v>25</v>
       </c>
-      <c r="W45" s="17" t="n">
+      <c r="W45" s="20" t="n">
         <v>0.001</v>
       </c>
       <c r="X45" s="11" t="n">
@@ -3303,14 +3321,14 @@
         <f aca="false">MAX(W33:W45)</f>
         <v>0.106</v>
       </c>
-      <c r="X47" s="16" t="n">
+      <c r="X47" s="19" t="n">
         <v>218</v>
       </c>
       <c r="Y47" s="0" t="n">
         <f aca="false">X47-X$41</f>
         <v>14</v>
       </c>
-      <c r="Z47" s="17" t="n">
+      <c r="Z47" s="20" t="n">
         <v>0.004</v>
       </c>
     </row>
@@ -3712,7 +3730,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10"/>
-      <c r="F104" s="19"/>
+      <c r="F104" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Changes for revised ESR manuscript
</commit_message>
<xml_diff>
--- a/data/iTURBO2_input_ash_experiment.xlsx
+++ b/data/iTURBO2_input_ash_experiment.xlsx
@@ -419,8 +419,8 @@
   </sheetPr>
   <dimension ref="A1:Z104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P30" activeCellId="0" sqref="P30:Q43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A64" activeCellId="0" sqref="A64:F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3609,34 +3609,174 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10"/>
+      <c r="A64" s="10" t="n">
+        <v>61</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10"/>
+      <c r="A65" s="10" t="n">
+        <v>62</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10"/>
+      <c r="A66" s="10" t="n">
+        <v>63</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10"/>
+      <c r="A67" s="10" t="n">
+        <v>64</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10"/>
+      <c r="A68" s="10" t="n">
+        <v>65</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="10"/>
+      <c r="A69" s="10" t="n">
+        <v>66</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="10"/>
+      <c r="A70" s="10" t="n">
+        <v>67</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="10"/>
+      <c r="A71" s="10" t="n">
+        <v>68</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="10"/>
+      <c r="A72" s="10" t="n">
+        <v>69</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="10"/>
+      <c r="A73" s="10" t="n">
+        <v>70</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="10"/>

</xml_diff>